<commit_message>
input file datatype corrected
</commit_message>
<xml_diff>
--- a/data/Fall2018/db1-7_all-timepoints-runs/db6/16-genes_27-edges_db6_Sigmoid_estimation_all-timepoints.xlsx
+++ b/data/Fall2018/db1-7_all-timepoints-runs/db6/16-genes_27-edges_db6_Sigmoid_estimation_all-timepoints.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6123F6-5A03-4A4B-9879-5836D81D0884}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="28770" windowHeight="6840" tabRatio="857" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11723" tabRatio="857" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="7" r:id="rId1"/>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="45">
   <si>
     <t>CIN5</t>
   </si>
@@ -169,242 +175,11 @@
   <si>
     <t>dhmo1</t>
   </si>
-  <si>
-    <t>-0.1381</t>
-  </si>
-  <si>
-    <t>0.3511</t>
-  </si>
-  <si>
-    <t>-0.732</t>
-  </si>
-  <si>
-    <t>-0.3947</t>
-  </si>
-  <si>
-    <t>0.7491</t>
-  </si>
-  <si>
-    <t>-0.2792</t>
-  </si>
-  <si>
-    <t>-0.2436</t>
-  </si>
-  <si>
-    <t>0.1581</t>
-  </si>
-  <si>
-    <t>1.0793</t>
-  </si>
-  <si>
-    <t>-1.8448</t>
-  </si>
-  <si>
-    <t>-0.383</t>
-  </si>
-  <si>
-    <t>0.2693</t>
-  </si>
-  <si>
-    <t>-0.2042</t>
-  </si>
-  <si>
-    <t>-0.4827</t>
-  </si>
-  <si>
-    <t>1.1346</t>
-  </si>
-  <si>
-    <t>-6.5772</t>
-  </si>
-  <si>
-    <t>0.3494</t>
-  </si>
-  <si>
-    <t>1.712</t>
-  </si>
-  <si>
-    <t>1.2921</t>
-  </si>
-  <si>
-    <t>-0.6312</t>
-  </si>
-  <si>
-    <t>0.1274</t>
-  </si>
-  <si>
-    <t>-1.251</t>
-  </si>
-  <si>
-    <t>1.117</t>
-  </si>
-  <si>
-    <t>2.584</t>
-  </si>
-  <si>
-    <t>1.4649</t>
-  </si>
-  <si>
-    <t>-0.7654</t>
-  </si>
-  <si>
-    <t>-1.1456</t>
-  </si>
-  <si>
-    <t>-0.9423</t>
-  </si>
-  <si>
-    <t>2.3352</t>
-  </si>
-  <si>
-    <t>-0.3518</t>
-  </si>
-  <si>
-    <t>0.5869</t>
-  </si>
-  <si>
-    <t>0.0341</t>
-  </si>
-  <si>
-    <t>1.4453</t>
-  </si>
-  <si>
-    <t>-0.5607</t>
-  </si>
-  <si>
-    <t>0.1712</t>
-  </si>
-  <si>
-    <t>-1.463</t>
-  </si>
-  <si>
-    <t>0.3025</t>
-  </si>
-  <si>
-    <t>-0.0617</t>
-  </si>
-  <si>
-    <t>2.2291</t>
-  </si>
-  <si>
-    <t>1.2958</t>
-  </si>
-  <si>
-    <t>1.5911</t>
-  </si>
-  <si>
-    <t>1.2566</t>
-  </si>
-  <si>
-    <t>-3.5699</t>
-  </si>
-  <si>
-    <t>-0.345</t>
-  </si>
-  <si>
-    <t>-0.705</t>
-  </si>
-  <si>
-    <t>-1.0257</t>
-  </si>
-  <si>
-    <t>-0.7514</t>
-  </si>
-  <si>
-    <t>-0.3681</t>
-  </si>
-  <si>
-    <t>1.0401</t>
-  </si>
-  <si>
-    <t>0.4422</t>
-  </si>
-  <si>
-    <t>1.8072</t>
-  </si>
-  <si>
-    <t>-0.8927</t>
-  </si>
-  <si>
-    <t>1.1069</t>
-  </si>
-  <si>
-    <t>0.3945</t>
-  </si>
-  <si>
-    <t>0.3325</t>
-  </si>
-  <si>
-    <t>0.6703</t>
-  </si>
-  <si>
-    <t>0.7164</t>
-  </si>
-  <si>
-    <t>0.3263</t>
-  </si>
-  <si>
-    <t>1.9784</t>
-  </si>
-  <si>
-    <t>-0.5489</t>
-  </si>
-  <si>
-    <t>-0.5302</t>
-  </si>
-  <si>
-    <t>0.016</t>
-  </si>
-  <si>
-    <t>-0.04</t>
-  </si>
-  <si>
-    <t>0.3902</t>
-  </si>
-  <si>
-    <t>0.2778</t>
-  </si>
-  <si>
-    <t>0.0835</t>
-  </si>
-  <si>
-    <t>0.3892</t>
-  </si>
-  <si>
-    <t>0.6028</t>
-  </si>
-  <si>
-    <t>2.5266</t>
-  </si>
-  <si>
-    <t>0.4041</t>
-  </si>
-  <si>
-    <t>0.0511</t>
-  </si>
-  <si>
-    <t>-0.5177</t>
-  </si>
-  <si>
-    <t>0.8398</t>
-  </si>
-  <si>
-    <t>2.3845</t>
-  </si>
-  <si>
-    <t>0.1525</t>
-  </si>
-  <si>
-    <t>1.0756</t>
-  </si>
-  <si>
-    <t>0.9658</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -452,12 +227,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -900,7 +681,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -909,6 +690,7 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="429">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1338,8 +1120,8 @@
     <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="291"/>
-    <cellStyle name="Normal 3" xfId="304"/>
+    <cellStyle name="Normal 2" xfId="291" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Normal 3" xfId="304" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1675,19 +1457,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1695,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -1703,7 +1485,7 @@
         <v>0.15759999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1711,7 +1493,7 @@
         <v>0.22359999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1719,7 +1501,7 @@
         <v>0.20100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -1727,7 +1509,7 @@
         <v>0.18479999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -1735,7 +1517,7 @@
         <v>0.1026</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1743,7 +1525,7 @@
         <v>0.19259999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1533,7 @@
         <v>0.32240000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1541,7 @@
         <v>0.27179999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1767,7 +1549,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1775,7 +1557,7 @@
         <v>0.21659999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -1783,7 +1565,7 @@
         <v>0.17119999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1791,7 +1573,7 @@
         <v>0.14599999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1799,7 +1581,7 @@
         <v>0.4078</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1807,7 +1589,7 @@
         <v>0.2772</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +1597,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1835,17 +1617,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1898,7 +1680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -1951,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -2004,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -2110,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -2163,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -2216,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -2269,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2375,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -2428,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -2481,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -2534,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -2587,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2640,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -2693,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -2746,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2765,7 +2547,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2784,7 +2566,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2815,18 +2597,18 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -2834,7 +2616,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2842,7 +2624,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2850,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2858,7 +2640,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2866,7 +2648,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2874,7 +2656,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -2882,7 +2664,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2890,7 +2672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -2898,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2906,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -2914,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -2922,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2930,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -2950,7 +2732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2973,7 +2755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -3065,17 +2847,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3083,7 +2865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -3091,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -3099,7 +2881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -3107,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -3115,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -3123,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -3131,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -3139,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -3147,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -3155,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -3163,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -3171,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -3179,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -3187,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -3195,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -3203,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -3222,19 +3004,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3242,7 +3024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -3250,7 +3032,7 @@
         <v>7.8799999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -3258,7 +3040,7 @@
         <v>0.1118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -3266,7 +3048,7 @@
         <v>0.10050000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -3274,7 +3056,7 @@
         <v>9.2399999999999996E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -3282,7 +3064,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -3290,7 +3072,7 @@
         <v>9.6299999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -3298,7 +3080,7 @@
         <v>0.16120000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -3306,7 +3088,7 @@
         <v>0.13589999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -3314,7 +3096,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -3322,7 +3104,7 @@
         <v>0.10829999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -3330,7 +3112,7 @@
         <v>8.5599999999999996E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -3338,7 +3120,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -3346,7 +3128,7 @@
         <v>0.2039</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -3354,7 +3136,7 @@
         <v>0.1386</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -3362,7 +3144,7 @@
         <v>0.14149999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -3382,19 +3164,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="24" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3468,7 +3250,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -3542,7 +3324,7 @@
         <v>-0.68430000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -3561,7 +3343,7 @@
       <c r="F3" s="7">
         <v>0.5827</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="7">
         <v>-0.3947</v>
       </c>
@@ -3586,7 +3368,7 @@
       <c r="O3" s="7">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="8"/>
       <c r="Q3" s="7">
         <v>0.26819999999999999</v>
       </c>
@@ -3612,7 +3394,7 @@
         <v>-0.31900000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -3686,7 +3468,7 @@
         <v>1.0625</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -3760,7 +3542,7 @@
         <v>1.3012999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -3834,7 +3616,7 @@
         <v>-1.2761</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -3908,7 +3690,7 @@
         <v>-1.1623000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -3982,7 +3764,7 @@
         <v>-1.4531000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -4056,7 +3838,7 @@
         <v>-1.0219</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -4130,7 +3912,7 @@
         <v>0.7853</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -4204,7 +3986,7 @@
         <v>1.3534999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -4278,7 +4060,7 @@
         <v>0.20930000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -4352,7 +4134,7 @@
         <v>1.2694000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -4426,7 +4208,7 @@
         <v>0.47389999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -4500,7 +4282,7 @@
         <v>3.7161</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -4574,7 +4356,7 @@
         <v>-0.95709999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -4614,7 +4396,7 @@
       <c r="M17" s="7">
         <v>1.3863000000000001</v>
       </c>
-      <c r="N17" s="7"/>
+      <c r="N17" s="8"/>
       <c r="O17" s="7">
         <v>0.45350000000000001</v>
       </c>
@@ -4658,19 +4440,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:T17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="21" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4735,15 +4519,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="7">
         <v>-1.361</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>45</v>
+      <c r="C2" s="2">
+        <v>-0.1381</v>
       </c>
       <c r="D2" s="7">
         <v>-1.1930000000000001</v>
@@ -4751,11 +4535,11 @@
       <c r="E2" s="7">
         <v>-1.4638</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>47</v>
+      <c r="F2" s="2">
+        <v>0.35110000000000002</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-0.73199999999999998</v>
       </c>
       <c r="H2" s="7">
         <v>-0.90820000000000001</v>
@@ -4787,8 +4571,8 @@
       <c r="Q2" s="7">
         <v>1.1315</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>48</v>
+      <c r="R2" s="2">
+        <v>-0.3947</v>
       </c>
       <c r="S2" s="7">
         <v>1.3111999999999999</v>
@@ -4800,15 +4584,15 @@
         <v>0.39219999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="7">
         <v>-0.17180000000000001</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>50</v>
+      <c r="C3" s="2">
+        <v>-0.2792</v>
       </c>
       <c r="D3" s="7">
         <v>-0.17519999999999999</v>
@@ -4816,16 +4600,16 @@
       <c r="E3" s="7">
         <v>-0.68840000000000001</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>52</v>
+      <c r="F3" s="2">
+        <v>-0.24360000000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.15809999999999999</v>
       </c>
       <c r="H3" s="7">
         <v>-0.42530000000000001</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="7">
         <v>0.56820000000000004</v>
       </c>
@@ -4850,8 +4634,8 @@
       <c r="Q3" s="7">
         <v>2.9009999999999998</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>53</v>
+      <c r="R3" s="2">
+        <v>1.0792999999999999</v>
       </c>
       <c r="S3" s="7">
         <v>0.89990000000000003</v>
@@ -4863,25 +4647,25 @@
         <v>-0.29010000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="7">
         <v>-0.66849999999999998</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="7">
         <v>-0.43219999999999997</v>
       </c>
       <c r="E4" s="7">
         <v>-0.1191</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>56</v>
+      <c r="F4" s="2">
+        <v>-0.38300000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.26929999999999998</v>
       </c>
       <c r="H4" s="7">
         <v>-7.5700000000000003E-2</v>
@@ -4889,7 +4673,7 @@
       <c r="I4" s="7">
         <v>0.59750000000000003</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="7">
         <v>-0.3216</v>
       </c>
@@ -4911,10 +4695,10 @@
       <c r="Q4" s="7">
         <v>0.55030000000000001</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="7"/>
+      <c r="R4" s="2">
+        <v>-0.20419999999999999</v>
+      </c>
+      <c r="S4" s="8"/>
       <c r="T4" s="7">
         <v>2.1099000000000001</v>
       </c>
@@ -4922,15 +4706,15 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="7">
         <v>1.0679000000000001</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>59</v>
+      <c r="C5" s="2">
+        <v>1.1346000000000001</v>
       </c>
       <c r="D5" s="7">
         <v>0.32869999999999999</v>
@@ -4938,11 +4722,11 @@
       <c r="E5" s="7">
         <v>1.0511999999999999</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>61</v>
+      <c r="F5" s="2">
+        <v>-6.5772000000000004</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.34939999999999999</v>
       </c>
       <c r="H5" s="7">
         <v>1.1438999999999999</v>
@@ -4950,7 +4734,7 @@
       <c r="I5" s="7">
         <v>-0.6613</v>
       </c>
-      <c r="J5" s="7"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="7">
         <v>8.5900000000000004E-2</v>
       </c>
@@ -4972,8 +4756,8 @@
       <c r="Q5" s="7">
         <v>1.0144</v>
       </c>
-      <c r="R5" s="7" t="s">
-        <v>62</v>
+      <c r="R5" s="2">
+        <v>1.712</v>
       </c>
       <c r="S5" s="7">
         <v>-1.3766</v>
@@ -4985,15 +4769,15 @@
         <v>0.99009999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="7">
         <v>-1.5613999999999999</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>64</v>
+      <c r="C6" s="2">
+        <v>-0.63119999999999998</v>
       </c>
       <c r="D6" s="7">
         <v>-1.9643999999999999</v>
@@ -5001,11 +4785,11 @@
       <c r="E6" s="7">
         <v>-2.0152000000000001</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>66</v>
+      <c r="F6" s="2">
+        <v>0.12740000000000001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-1.2509999999999999</v>
       </c>
       <c r="H6" s="7">
         <v>-1.7951999999999999</v>
@@ -5037,8 +4821,8 @@
       <c r="Q6" s="7">
         <v>-1.8407</v>
       </c>
-      <c r="R6" s="7" t="s">
-        <v>67</v>
+      <c r="R6" s="2">
+        <v>1.117</v>
       </c>
       <c r="S6" s="7">
         <v>1.4206000000000001</v>
@@ -5050,15 +4834,15 @@
         <v>-2.7338</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="7">
         <v>-0.3155</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>69</v>
+      <c r="C7" s="2">
+        <v>1.4649000000000001</v>
       </c>
       <c r="D7" s="7">
         <v>-0.80289999999999995</v>
@@ -5066,11 +4850,11 @@
       <c r="E7" s="7">
         <v>0.5141</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>71</v>
+      <c r="F7" s="2">
+        <v>-0.76539999999999997</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-1.1456</v>
       </c>
       <c r="H7" s="7">
         <v>0.50960000000000005</v>
@@ -5102,8 +4886,8 @@
       <c r="Q7" s="7">
         <v>-0.5786</v>
       </c>
-      <c r="R7" s="7" t="s">
-        <v>72</v>
+      <c r="R7" s="2">
+        <v>-0.94230000000000003</v>
       </c>
       <c r="S7" s="7">
         <v>0.78710000000000002</v>
@@ -5115,15 +4899,15 @@
         <v>0.14269999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="7">
         <v>0.96209999999999996</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>74</v>
+      <c r="C8" s="2">
+        <v>-0.3518</v>
       </c>
       <c r="D8" s="7">
         <v>0.31009999999999999</v>
@@ -5131,11 +4915,11 @@
       <c r="E8" s="7">
         <v>-0.15890000000000001</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>76</v>
+      <c r="F8" s="2">
+        <v>0.58689999999999998</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3.4099999999999998E-2</v>
       </c>
       <c r="H8" s="7">
         <v>0.48599999999999999</v>
@@ -5167,8 +4951,8 @@
       <c r="Q8" s="7">
         <v>-2.6499999999999999E-2</v>
       </c>
-      <c r="R8" s="7" t="s">
-        <v>77</v>
+      <c r="R8" s="2">
+        <v>1.4453</v>
       </c>
       <c r="S8" s="7">
         <v>-1.0232000000000001</v>
@@ -5180,15 +4964,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="7">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>79</v>
+      <c r="C9" s="2">
+        <v>0.17119999999999999</v>
       </c>
       <c r="D9" s="7">
         <v>-1.9531000000000001</v>
@@ -5196,11 +4980,11 @@
       <c r="E9" s="7">
         <v>-0.21510000000000001</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>81</v>
+      <c r="F9" s="2">
+        <v>-1.4630000000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.30249999999999999</v>
       </c>
       <c r="H9" s="7">
         <v>-2.2646000000000002</v>
@@ -5232,8 +5016,8 @@
       <c r="Q9" s="7">
         <v>-1.2024999999999999</v>
       </c>
-      <c r="R9" s="7" t="s">
-        <v>82</v>
+      <c r="R9" s="2">
+        <v>-6.1699999999999998E-2</v>
       </c>
       <c r="S9" s="7">
         <v>1.1213</v>
@@ -5245,15 +5029,15 @@
         <v>1.583</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="7">
         <v>-0.91690000000000005</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>84</v>
+      <c r="C10" s="2">
+        <v>1.2958000000000001</v>
       </c>
       <c r="D10" s="7">
         <v>0.42699999999999999</v>
@@ -5261,11 +5045,11 @@
       <c r="E10" s="7">
         <v>-7.1199999999999999E-2</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>86</v>
+      <c r="F10" s="2">
+        <v>1.5911</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.2565999999999999</v>
       </c>
       <c r="H10" s="7">
         <v>0.39100000000000001</v>
@@ -5297,8 +5081,8 @@
       <c r="Q10" s="7">
         <v>1.099</v>
       </c>
-      <c r="R10" s="7" t="s">
-        <v>87</v>
+      <c r="R10" s="2">
+        <v>-3.5699000000000001</v>
       </c>
       <c r="S10" s="7">
         <v>-1.8355999999999999</v>
@@ -5310,15 +5094,15 @@
         <v>-2.9781</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="7">
         <v>-0.87239999999999995</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>89</v>
+      <c r="C11" s="2">
+        <v>-0.70499999999999996</v>
       </c>
       <c r="D11" s="7">
         <v>-1.5949</v>
@@ -5326,11 +5110,11 @@
       <c r="E11" s="7">
         <v>-1.7487999999999999</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>91</v>
+      <c r="F11" s="2">
+        <v>-1.0257000000000001</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-0.75139999999999996</v>
       </c>
       <c r="H11" s="7">
         <v>-1.4853000000000001</v>
@@ -5362,8 +5146,8 @@
       <c r="Q11" s="7">
         <v>-1.5888</v>
       </c>
-      <c r="R11" s="7" t="s">
-        <v>92</v>
+      <c r="R11" s="2">
+        <v>-0.36809999999999998</v>
       </c>
       <c r="S11" s="7">
         <v>1.5089999999999999</v>
@@ -5375,15 +5159,15 @@
         <v>-0.70409999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="7">
         <v>0.48080000000000001</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>94</v>
+      <c r="C12" s="2">
+        <v>0.44219999999999998</v>
       </c>
       <c r="D12" s="7">
         <v>1.4923999999999999</v>
@@ -5391,11 +5175,11 @@
       <c r="E12" s="7">
         <v>2.4096000000000002</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>96</v>
+      <c r="F12" s="2">
+        <v>1.8071999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-0.89270000000000005</v>
       </c>
       <c r="H12" s="7">
         <v>0.75890000000000002</v>
@@ -5427,26 +5211,26 @@
       <c r="Q12" s="7">
         <v>0.5645</v>
       </c>
-      <c r="R12" s="7" t="s">
-        <v>97</v>
+      <c r="R12" s="2">
+        <v>1.1069</v>
       </c>
       <c r="S12" s="7">
         <v>0.4713</v>
       </c>
-      <c r="T12" s="7"/>
+      <c r="T12" s="8"/>
       <c r="U12" s="7">
         <v>1.2195</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="7">
         <v>9.8199999999999996E-2</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>99</v>
+      <c r="C13" s="2">
+        <v>0.33250000000000002</v>
       </c>
       <c r="D13" s="7">
         <v>0.29420000000000002</v>
@@ -5454,11 +5238,11 @@
       <c r="E13" s="7">
         <v>5.2299999999999999E-2</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>101</v>
+      <c r="F13" s="2">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.71640000000000004</v>
       </c>
       <c r="H13" s="7">
         <v>0.33739999999999998</v>
@@ -5484,12 +5268,12 @@
       <c r="O13" s="7">
         <v>0.65690000000000004</v>
       </c>
-      <c r="P13" s="7"/>
+      <c r="P13" s="8"/>
       <c r="Q13" s="7">
         <v>-0.36409999999999998</v>
       </c>
-      <c r="R13" s="7" t="s">
-        <v>102</v>
+      <c r="R13" s="2">
+        <v>0.32629999999999998</v>
       </c>
       <c r="S13" s="7">
         <v>-0.1216</v>
@@ -5501,13 +5285,13 @@
         <v>-0.113</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="s">
-        <v>104</v>
+      <c r="B14" s="8"/>
+      <c r="C14" s="2">
+        <v>-0.54890000000000005</v>
       </c>
       <c r="D14" s="7">
         <v>0.24909999999999999</v>
@@ -5515,11 +5299,11 @@
       <c r="E14" s="7">
         <v>0.90359999999999996</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>106</v>
+      <c r="F14" s="2">
+        <v>-0.5302</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.6E-2</v>
       </c>
       <c r="H14" s="7">
         <v>-9.9699999999999997E-2</v>
@@ -5551,8 +5335,8 @@
       <c r="Q14" s="7">
         <v>0.41470000000000001</v>
       </c>
-      <c r="R14" s="7" t="s">
-        <v>107</v>
+      <c r="R14" s="2">
+        <v>-0.04</v>
       </c>
       <c r="S14" s="7">
         <v>-0.1053</v>
@@ -5564,25 +5348,25 @@
         <v>1.0256000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="7">
         <v>0.5524</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="7">
         <v>1.3068</v>
       </c>
       <c r="E15" s="7">
         <v>1.5691999999999999</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>110</v>
+      <c r="F15" s="2">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="G15" s="2">
+        <v>8.3500000000000005E-2</v>
       </c>
       <c r="H15" s="7">
         <v>2.1132</v>
@@ -5614,8 +5398,8 @@
       <c r="Q15" s="7">
         <v>-0.34839999999999999</v>
       </c>
-      <c r="R15" s="7" t="s">
-        <v>111</v>
+      <c r="R15" s="2">
+        <v>0.38919999999999999</v>
       </c>
       <c r="S15" s="7">
         <v>0.86570000000000003</v>
@@ -5627,25 +5411,25 @@
         <v>1.3242</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="7">
         <v>-0.4763</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="7">
         <v>-0.33360000000000001</v>
       </c>
       <c r="E16" s="7">
         <v>-0.54890000000000005</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>114</v>
+      <c r="F16" s="2">
+        <v>2.5266000000000002</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.40410000000000001</v>
       </c>
       <c r="H16" s="7">
         <v>2.5700000000000001E-2</v>
@@ -5677,8 +5461,8 @@
       <c r="Q16" s="7">
         <v>-7.9000000000000008E-3</v>
       </c>
-      <c r="R16" s="7" t="s">
-        <v>115</v>
+      <c r="R16" s="2">
+        <v>5.11E-2</v>
       </c>
       <c r="S16" s="7">
         <v>0.57050000000000001</v>
@@ -5690,15 +5474,15 @@
         <v>-0.24779999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="7">
         <v>0.83440000000000003</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>117</v>
+      <c r="C17" s="2">
+        <v>0.83979999999999999</v>
       </c>
       <c r="D17" s="7">
         <v>0.91839999999999999</v>
@@ -5706,11 +5490,11 @@
       <c r="E17" s="7">
         <v>0.47470000000000001</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>119</v>
+      <c r="F17" s="2">
+        <v>2.3845000000000001</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.1525</v>
       </c>
       <c r="H17" s="7">
         <v>0.65110000000000001</v>
@@ -5742,13 +5526,13 @@
       <c r="Q17" s="7">
         <v>0.61909999999999998</v>
       </c>
-      <c r="R17" s="7" t="s">
-        <v>120</v>
+      <c r="R17" s="2">
+        <v>1.0755999999999999</v>
       </c>
       <c r="S17" s="7">
         <v>0.1502</v>
       </c>
-      <c r="T17" s="7"/>
+      <c r="T17" s="8"/>
       <c r="U17" s="7">
         <v>-4.1300000000000003E-2</v>
       </c>
@@ -5765,19 +5549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="21" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -5842,7 +5628,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -5894,10 +5680,10 @@
       <c r="Q2" s="7">
         <v>1.3557999999999999</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="7"/>
+      <c r="R2" s="2">
+        <v>0.74909999999999999</v>
+      </c>
+      <c r="S2" s="8"/>
       <c r="T2" s="7">
         <v>0.62609999999999999</v>
       </c>
@@ -5905,7 +5691,7 @@
         <v>1.1281000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -5957,8 +5743,8 @@
       <c r="Q3" s="7">
         <v>2.0644</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>54</v>
+      <c r="R3" s="2">
+        <v>-1.8448</v>
       </c>
       <c r="S3" s="7">
         <v>4.2244000000000002</v>
@@ -5970,7 +5756,7 @@
         <v>0.35189999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -6022,8 +5808,8 @@
       <c r="Q4" s="7">
         <v>2.3325</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>58</v>
+      <c r="R4" s="2">
+        <v>-0.48270000000000002</v>
       </c>
       <c r="S4" s="7">
         <v>1.7847999999999999</v>
@@ -6035,7 +5821,7 @@
         <v>5.1330999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -6087,18 +5873,18 @@
       <c r="Q5" s="7">
         <v>-2.1700000000000001E-2</v>
       </c>
-      <c r="R5" s="7" t="s">
-        <v>63</v>
+      <c r="R5" s="2">
+        <v>1.2921</v>
       </c>
       <c r="S5" s="7">
         <v>0.25700000000000001</v>
       </c>
-      <c r="T5" s="7"/>
+      <c r="T5" s="8"/>
       <c r="U5" s="7">
         <v>0.51270000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -6150,8 +5936,8 @@
       <c r="Q6" s="7">
         <v>0.22900000000000001</v>
       </c>
-      <c r="R6" s="7" t="s">
-        <v>68</v>
+      <c r="R6" s="2">
+        <v>2.5840000000000001</v>
       </c>
       <c r="S6" s="7">
         <v>-0.10780000000000001</v>
@@ -6163,7 +5949,7 @@
         <v>-1.0476000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -6179,7 +5965,7 @@
       <c r="E7" s="7">
         <v>-6.1600000000000002E-2</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="7">
         <v>-0.19980000000000001</v>
       </c>
@@ -6213,8 +5999,8 @@
       <c r="Q7" s="7">
         <v>-0.92279999999999995</v>
       </c>
-      <c r="R7" s="7" t="s">
-        <v>73</v>
+      <c r="R7" s="2">
+        <v>2.3351999999999999</v>
       </c>
       <c r="S7" s="7">
         <v>-0.33929999999999999</v>
@@ -6226,7 +6012,7 @@
         <v>-0.61240000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -6278,8 +6064,8 @@
       <c r="Q8" s="7">
         <v>0.48330000000000001</v>
       </c>
-      <c r="R8" s="7" t="s">
-        <v>78</v>
+      <c r="R8" s="2">
+        <v>-0.56069999999999998</v>
       </c>
       <c r="S8" s="7">
         <v>3.3700000000000001E-2</v>
@@ -6291,7 +6077,7 @@
         <v>-0.97250000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -6343,8 +6129,8 @@
       <c r="Q9" s="7">
         <v>-0.86240000000000006</v>
       </c>
-      <c r="R9" s="7" t="s">
-        <v>83</v>
+      <c r="R9" s="2">
+        <v>2.2290999999999999</v>
       </c>
       <c r="S9" s="7">
         <v>1.0261</v>
@@ -6356,7 +6142,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -6408,8 +6194,8 @@
       <c r="Q10" s="7">
         <v>2.133</v>
       </c>
-      <c r="R10" s="7" t="s">
-        <v>88</v>
+      <c r="R10" s="2">
+        <v>-0.34499999999999997</v>
       </c>
       <c r="S10" s="7">
         <v>-2.0594999999999999</v>
@@ -6421,7 +6207,7 @@
         <v>-2.0489000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -6473,8 +6259,8 @@
       <c r="Q11" s="7">
         <v>0.90580000000000005</v>
       </c>
-      <c r="R11" s="7" t="s">
-        <v>93</v>
+      <c r="R11" s="2">
+        <v>1.0401</v>
       </c>
       <c r="S11" s="7">
         <v>0.37530000000000002</v>
@@ -6486,18 +6272,18 @@
         <v>-0.30449999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="7">
         <v>6.0278999999999998</v>
       </c>
       <c r="D12" s="7">
         <v>-0.84640000000000004</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="7">
         <v>0.94030000000000002</v>
       </c>
@@ -6507,31 +6293,31 @@
       <c r="H12" s="7">
         <v>1.6552</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="7">
         <v>2.3471000000000002</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="7">
         <v>-1.4205000000000001</v>
       </c>
       <c r="N12" s="7">
         <v>-0.37619999999999998</v>
       </c>
-      <c r="O12" s="7"/>
+      <c r="O12" s="8"/>
       <c r="P12" s="7">
         <v>-0.82179999999999997</v>
       </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q12" s="8"/>
+      <c r="R12" s="2">
+        <v>0.39450000000000002</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -6583,8 +6369,8 @@
       <c r="Q13" s="7">
         <v>-2.5100000000000001E-2</v>
       </c>
-      <c r="R13" s="7" t="s">
-        <v>103</v>
+      <c r="R13" s="2">
+        <v>1.9783999999999999</v>
       </c>
       <c r="S13" s="7">
         <v>0.24010000000000001</v>
@@ -6596,7 +6382,7 @@
         <v>-0.77039999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -6636,7 +6422,7 @@
       <c r="M14" s="7">
         <v>-0.28699999999999998</v>
       </c>
-      <c r="N14" s="7"/>
+      <c r="N14" s="8"/>
       <c r="O14" s="7">
         <v>0.4501</v>
       </c>
@@ -6646,8 +6432,8 @@
       <c r="Q14" s="7">
         <v>2.1431</v>
       </c>
-      <c r="R14" s="7" t="s">
-        <v>108</v>
+      <c r="R14" s="2">
+        <v>0.39019999999999999</v>
       </c>
       <c r="S14" s="7">
         <v>-0.41870000000000002</v>
@@ -6659,7 +6445,7 @@
         <v>0.55079999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -6672,7 +6458,7 @@
       <c r="D15" s="7">
         <v>1.8004</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="7">
         <v>1.9258999999999999</v>
       </c>
@@ -6709,8 +6495,8 @@
       <c r="Q15" s="7">
         <v>-0.94869999999999999</v>
       </c>
-      <c r="R15" s="7" t="s">
-        <v>112</v>
+      <c r="R15" s="2">
+        <v>0.6028</v>
       </c>
       <c r="S15" s="7">
         <v>-0.85270000000000001</v>
@@ -6722,7 +6508,7 @@
         <v>0.87580000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -6774,8 +6560,8 @@
       <c r="Q16" s="7">
         <v>0.21049999999999999</v>
       </c>
-      <c r="R16" s="7" t="s">
-        <v>116</v>
+      <c r="R16" s="2">
+        <v>-0.51770000000000005</v>
       </c>
       <c r="S16" s="7">
         <v>-0.45090000000000002</v>
@@ -6787,7 +6573,7 @@
         <v>-0.222</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -6797,7 +6583,7 @@
       <c r="C17" s="7">
         <v>-0.22620000000000001</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="7">
         <v>0.40500000000000003</v>
       </c>
@@ -6807,7 +6593,7 @@
       <c r="G17" s="7">
         <v>1.7576000000000001</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="7">
         <v>1.3798999999999999</v>
       </c>
@@ -6820,19 +6606,19 @@
       <c r="L17" s="7">
         <v>-1.0851999999999999</v>
       </c>
-      <c r="M17" s="7"/>
+      <c r="M17" s="8"/>
       <c r="N17" s="7">
         <v>-0.86339999999999995</v>
       </c>
-      <c r="O17" s="7"/>
+      <c r="O17" s="8"/>
       <c r="P17" s="7">
         <v>0.2954</v>
       </c>
       <c r="Q17" s="7">
         <v>0.50780000000000003</v>
       </c>
-      <c r="R17" s="7" t="s">
-        <v>121</v>
+      <c r="R17" s="2">
+        <v>0.96579999999999999</v>
       </c>
       <c r="S17" s="7">
         <v>6.6299999999999998E-2</v>
@@ -6856,19 +6642,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" activeCellId="2" sqref="C17 I16 N17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="19" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -6927,7 +6715,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -6986,7 +6774,7 @@
         <v>1.6383000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -7045,7 +6833,7 @@
         <v>-0.58099999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -7104,7 +6892,7 @@
         <v>0.50570000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -7163,7 +6951,7 @@
         <v>-1.6099000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -7222,7 +7010,7 @@
         <v>-0.90780000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -7281,7 +7069,7 @@
         <v>-0.42020000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -7340,7 +7128,7 @@
         <v>-0.91920000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -7399,7 +7187,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -7458,7 +7246,7 @@
         <v>-5.5450999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -7517,7 +7305,7 @@
         <v>1.7020999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -7576,7 +7364,7 @@
         <v>-0.68049999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -7635,7 +7423,7 @@
         <v>-0.1706</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -7694,7 +7482,7 @@
         <v>0.56089999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -7753,7 +7541,7 @@
         <v>1.2277</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -7778,7 +7566,7 @@
       <c r="H16" s="7">
         <v>-0.1171</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="7">
         <v>0.3775</v>
       </c>
@@ -7810,14 +7598,14 @@
         <v>-1.0305</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="7">
         <v>-1.903</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="7">
         <v>1.5545</v>
       </c>
@@ -7848,7 +7636,7 @@
       <c r="M17" s="7">
         <v>-0.5958</v>
       </c>
-      <c r="N17" s="7"/>
+      <c r="N17" s="8"/>
       <c r="O17" s="7">
         <v>-1.0683</v>
       </c>
@@ -7877,19 +7665,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="21" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -7954,7 +7742,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -8019,7 +7807,7 @@
         <v>0.69110000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -8084,7 +7872,7 @@
         <v>0.57740000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8149,7 +7937,7 @@
         <v>-0.92689999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -8214,7 +8002,7 @@
         <v>-5.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -8279,7 +8067,7 @@
         <v>-2.0002</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -8344,7 +8132,7 @@
         <v>-1.0406</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -8409,7 +8197,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -8474,7 +8262,7 @@
         <v>0.47910000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -8539,7 +8327,7 @@
         <v>-2.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -8604,7 +8392,7 @@
         <v>1.4575</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -8669,7 +8457,7 @@
         <v>-2.0543999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -8734,7 +8522,7 @@
         <v>0.1542</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -8799,7 +8587,7 @@
         <v>1.0784</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -8864,7 +8652,7 @@
         <v>-0.15740000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -8929,7 +8717,7 @@
         <v>0.1336</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -9006,19 +8794,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="21" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -9083,7 +8871,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -9148,7 +8936,7 @@
         <v>0.69069999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -9213,11 +9001,11 @@
         <v>0.1575</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="7">
         <v>2.4161999999999999</v>
       </c>
@@ -9276,7 +9064,7 @@
         <v>1.4026000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -9289,8 +9077,8 @@
       <c r="D5" s="7">
         <v>0.64429999999999998</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="7">
         <v>1.2698</v>
       </c>
@@ -9312,7 +9100,7 @@
       <c r="M5" s="7">
         <v>1.7876000000000001</v>
       </c>
-      <c r="N5" s="7"/>
+      <c r="N5" s="8"/>
       <c r="O5" s="7">
         <v>-1.1853</v>
       </c>
@@ -9335,7 +9123,7 @@
         <v>-1.5194000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -9400,7 +9188,7 @@
         <v>-0.26669999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -9465,7 +9253,7 @@
         <v>-0.3397</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -9530,7 +9318,7 @@
         <v>-0.55430000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -9595,7 +9383,7 @@
         <v>-8.2600000000000007E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -9660,7 +9448,7 @@
         <v>-1.9366000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -9725,7 +9513,7 @@
         <v>0.79010000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -9774,17 +9562,17 @@
       <c r="P12" s="7">
         <v>0.15559999999999999</v>
       </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
       <c r="S12" s="7">
         <v>1.1749000000000001</v>
       </c>
       <c r="T12" s="7">
         <v>0.75049999999999994</v>
       </c>
-      <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U12" s="8"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -9849,7 +9637,7 @@
         <v>0.14729999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -9914,7 +9702,7 @@
         <v>1.5842000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -9979,7 +9767,7 @@
         <v>1.7755000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -10044,11 +9832,11 @@
         <v>-6.7799999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="7">
         <v>0.12870000000000001</v>
       </c>
@@ -10070,7 +9858,7 @@
       <c r="I17" s="7">
         <v>-0.23730000000000001</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="8"/>
       <c r="K17" s="7">
         <v>0.69140000000000001</v>
       </c>
@@ -10092,7 +9880,7 @@
       <c r="Q17" s="7">
         <v>0.25569999999999998</v>
       </c>
-      <c r="R17" s="7"/>
+      <c r="R17" s="8"/>
       <c r="S17" s="7">
         <v>0.40379999999999999</v>
       </c>
@@ -10115,17 +9903,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -10178,7 +9966,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -10231,7 +10019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -10284,7 +10072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -10337,7 +10125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -10390,7 +10178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -10443,7 +10231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -10496,7 +10284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -10549,7 +10337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -10602,7 +10390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -10655,7 +10443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -10708,7 +10496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -10761,7 +10549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -10814,7 +10602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -10867,7 +10655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -10920,7 +10708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -10973,7 +10761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>

</xml_diff>